<commit_message>
Reroute RZV vaccine file in the scripts to keep the consistancey
</commit_message>
<xml_diff>
--- a/docs/manuscript/Table 1.xlsx
+++ b/docs/manuscript/Table 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\HPRU\Shingrix\HPRU_RZV\docs\tabs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD9D65-3151-4685-8A32-BD000E04D685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2A0929-AA43-426C-A886-09BD62619E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -387,6 +387,12 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -401,12 +407,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0A42E2-CD23-4C67-BA97-748E6A031FBF}">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="T32" sqref="T32:AI37"/>
     </sheetView>
   </sheetViews>
@@ -728,26 +728,26 @@
       <c r="D1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24" t="s">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24" t="s">
+      <c r="J1" s="26"/>
+      <c r="K1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="25" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="25"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="8" t="s">
         <v>18</v>
       </c>
@@ -887,39 +887,39 @@
       </c>
       <c r="I3" s="17">
         <f>-Z3</f>
-        <v>34960.520427313</v>
+        <v>33706.0578608129</v>
       </c>
       <c r="J3" s="19">
         <f>AF3</f>
-        <v>0.54961601944385197</v>
+        <v>0.54679755127354501</v>
       </c>
       <c r="K3" s="17">
         <f>AB3</f>
-        <v>3296.75701117668</v>
+        <v>3186.60962820637</v>
       </c>
       <c r="L3" s="19">
         <f>AG3</f>
-        <v>0.51449079570792999</v>
+        <v>0.51115069742946195</v>
       </c>
       <c r="M3" s="20">
         <f>-AA3/1000000</f>
-        <v>6.5291961903377498</v>
+        <v>6.2360332324265695</v>
       </c>
       <c r="N3" s="19">
         <f>AH3</f>
-        <v>0.47824346520466698</v>
+        <v>0.47407751644561502</v>
       </c>
       <c r="O3" s="20">
         <f>AC3</f>
-        <v>117.42194790004</v>
+        <v>113.377224862967</v>
       </c>
       <c r="P3" s="20">
         <f>(K3 * 20 + M3 * 1000) /G3</f>
-        <v>117.42194790004029</v>
+        <v>113.37722486296749</v>
       </c>
       <c r="Q3" s="18">
         <f>E3/I3*1000</f>
-        <v>8.8260656671607691</v>
+        <v>9.1545516928670647</v>
       </c>
       <c r="S3" t="s">
         <v>49</v>
@@ -943,16 +943,16 @@
         <v>617127.69809915998</v>
       </c>
       <c r="Z3">
-        <v>-34960.520427313</v>
+        <v>-33706.0578608129</v>
       </c>
       <c r="AA3">
-        <v>-6529196.1903377501</v>
+        <v>-6236033.2324265698</v>
       </c>
       <c r="AB3">
-        <v>3296.75701117668</v>
+        <v>3186.60962820637</v>
       </c>
       <c r="AC3">
-        <v>117.42194790004</v>
+        <v>113.377224862967</v>
       </c>
       <c r="AD3">
         <v>0.50216009675581297</v>
@@ -961,20 +961,20 @@
         <v>0.50216009675581297</v>
       </c>
       <c r="AF3">
-        <v>0.54961601944385197</v>
+        <v>0.54679755127354501</v>
       </c>
       <c r="AG3">
-        <v>0.51449079570792999</v>
+        <v>0.51115069742946195</v>
       </c>
       <c r="AH3">
-        <v>0.47824346520466698</v>
+        <v>0.47407751644561502</v>
       </c>
       <c r="AI3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="15" t="str">
@@ -1007,39 +1007,39 @@
       </c>
       <c r="I4" s="17">
         <f t="shared" ref="I4:I5" si="6">-Z4</f>
-        <v>23537.7042656339</v>
+        <v>22908.903181728401</v>
       </c>
       <c r="J4" s="19">
         <f t="shared" ref="J4:J5" si="7">AF4</f>
-        <v>0.91965339781243904</v>
+        <v>0.91843793158320297</v>
       </c>
       <c r="K4" s="17">
         <f t="shared" ref="K4:K5" si="8">AB4</f>
-        <v>2504.4179026765901</v>
+        <v>2450.0437441876402</v>
       </c>
       <c r="L4" s="19">
         <f t="shared" ref="L4:L5" si="9">AG4</f>
-        <v>0.90532941534686096</v>
+        <v>0.90415194787729403</v>
       </c>
       <c r="M4" s="20">
         <f t="shared" ref="M4:M5" si="10">-AA4/1000000</f>
-        <v>5.5692610116056906</v>
+        <v>5.3964384847435598</v>
       </c>
       <c r="N4" s="19">
         <f t="shared" ref="N4:N5" si="11">AH4</f>
-        <v>0.88617464190312401</v>
+        <v>0.88432711890054905</v>
       </c>
       <c r="O4" s="20">
         <f t="shared" ref="O4:O5" si="12">AC4</f>
-        <v>116.471281665232</v>
+        <v>113.056452248063</v>
       </c>
       <c r="P4" s="20">
         <f>(K4 * 20 + M4 * 1000) /G4</f>
-        <v>115.25637354499503</v>
+        <v>112.64651946584451</v>
       </c>
       <c r="Q4" s="18">
         <f t="shared" ref="Q4:Q5" si="13">E4/I4*1000</f>
-        <v>10.258068048942301</v>
+        <v>10.539630385505664</v>
       </c>
       <c r="S4" t="s">
         <v>50</v>
@@ -1063,16 +1063,16 @@
         <v>482902.74414550501</v>
       </c>
       <c r="Z4">
-        <v>-23537.7042656339</v>
+        <v>-22908.903181728401</v>
       </c>
       <c r="AA4">
-        <v>-5569261.0116056902</v>
+        <v>-5396438.4847435597</v>
       </c>
       <c r="AB4">
-        <v>2504.4179026765901</v>
+        <v>2450.0437441876402</v>
       </c>
       <c r="AC4">
-        <v>116.471281665232</v>
+        <v>113.056452248063</v>
       </c>
       <c r="AD4">
         <v>0.89510063316451904</v>
@@ -1081,20 +1081,20 @@
         <v>0.89510063316451904</v>
       </c>
       <c r="AF4">
-        <v>0.91965339781243904</v>
+        <v>0.91843793158320297</v>
       </c>
       <c r="AG4">
-        <v>0.90532941534686096</v>
+        <v>0.90415194787729403</v>
       </c>
       <c r="AH4">
-        <v>0.88617464190312401</v>
+        <v>0.88432711890054905</v>
       </c>
       <c r="AI4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="15" t="str">
         <f t="shared" si="1"/>
         <v>[75,80)</v>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="I5" s="17">
         <f t="shared" si="6"/>
-        <v>5110.76629441356</v>
+        <v>5027.7031981967202</v>
       </c>
       <c r="J5" s="19">
         <f t="shared" si="7"/>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="K5" s="17">
         <f t="shared" si="8"/>
-        <v>606.63070420527004</v>
+        <v>597.53479213669596</v>
       </c>
       <c r="L5" s="19">
         <f t="shared" si="9"/>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="M5" s="20">
         <f t="shared" si="10"/>
-        <v>1.5539952942836301</v>
+        <v>1.5215653676954</v>
       </c>
       <c r="N5" s="19">
         <f t="shared" si="11"/>
@@ -1149,15 +1149,15 @@
       </c>
       <c r="O5" s="20">
         <f t="shared" si="12"/>
-        <v>115.390384954252</v>
+        <v>112.15935273421699</v>
       </c>
       <c r="P5" s="20">
         <f>(K5 * 20 + M5 * 1000) /G5</f>
-        <v>106.16715168249242</v>
+        <v>104.50445102146709</v>
       </c>
       <c r="Q5" s="18">
         <f t="shared" si="13"/>
-        <v>12.612166308494679</v>
+        <v>12.820532940789326</v>
       </c>
       <c r="S5" t="s">
         <v>50</v>
@@ -1181,16 +1181,16 @@
         <v>128915.668937985</v>
       </c>
       <c r="Z5">
-        <v>-5110.76629441356</v>
+        <v>-5027.7031981967202</v>
       </c>
       <c r="AA5">
-        <v>-1553995.2942836301</v>
+        <v>-1521565.3676954</v>
       </c>
       <c r="AB5">
-        <v>606.63070420527004</v>
+        <v>597.53479213669596</v>
       </c>
       <c r="AC5">
-        <v>115.390384954252</v>
+        <v>112.15935273421699</v>
       </c>
       <c r="AD5">
         <v>1</v>
@@ -1231,23 +1231,23 @@
       <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="18"/>
     </row>
@@ -1255,11 +1255,11 @@
       <c r="A8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="27" t="str">
+      <c r="B8" s="22" t="str">
         <f>T8</f>
         <v>[80,85)</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="23">
         <f>V8/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -1285,39 +1285,39 @@
       </c>
       <c r="I8" s="17">
         <f t="shared" ref="I8:I13" si="18">-Z8</f>
-        <v>6145.9350657163704</v>
+        <v>6708.3275629876898</v>
       </c>
       <c r="J8" s="19">
         <f t="shared" ref="J8:J13" si="19">AF8</f>
-        <v>1.0966205401204601</v>
+        <v>1.1088260484132999</v>
       </c>
       <c r="K8" s="17">
         <f t="shared" ref="K8:K13" si="20">AB8</f>
-        <v>615.55938715145805</v>
+        <v>666.251075773612</v>
       </c>
       <c r="L8" s="19">
         <f t="shared" ref="L8:L13" si="21">AG8</f>
-        <v>1.0960639919252</v>
+        <v>1.10687054323516</v>
       </c>
       <c r="M8" s="20">
         <f t="shared" ref="M8:M13" si="22">-AA8/1000000</f>
-        <v>1.86099182972738</v>
+        <v>2.0280589322651998</v>
       </c>
       <c r="N8" s="19">
         <f t="shared" ref="N8:N13" si="23">AH8</f>
-        <v>1.1363119066147001</v>
+        <v>1.1541776809036499</v>
       </c>
       <c r="O8" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K8)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M8)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G8))</f>
-        <v>113.41880865032371</v>
+        <v>111.39020564710226</v>
       </c>
       <c r="P8" s="20">
         <f>(K8 * 20 + M8 * 1000) /G8</f>
-        <v>96.859180734945028</v>
+        <v>104.92999939008729</v>
       </c>
       <c r="Q8" s="18">
         <f t="shared" ref="Q8:Q13" si="24">E8/I8*1000</f>
-        <v>23.807176284768676</v>
+        <v>21.811302171876292</v>
       </c>
       <c r="S8" t="s">
         <v>51</v>
@@ -1341,16 +1341,16 @@
         <v>146317.359544251</v>
       </c>
       <c r="Z8">
-        <v>-6145.9350657163704</v>
+        <v>-6708.3275629876898</v>
       </c>
       <c r="AA8">
-        <v>-1860991.8297273801</v>
+        <v>-2028058.9322652</v>
       </c>
       <c r="AB8">
-        <v>615.55938715145805</v>
+        <v>666.251075773612</v>
       </c>
       <c r="AC8">
-        <v>113.418808650323</v>
+        <v>111.39020564710199</v>
       </c>
       <c r="AD8">
         <v>1.2381184304386501</v>
@@ -1359,13 +1359,13 @@
         <v>1.1190592152193199</v>
       </c>
       <c r="AF8">
-        <v>1.0966205401204601</v>
+        <v>1.1088260484132999</v>
       </c>
       <c r="AG8">
-        <v>1.0960639919252</v>
+        <v>1.10687054323516</v>
       </c>
       <c r="AH8">
-        <v>1.1363119066147001</v>
+        <v>1.1541776809036499</v>
       </c>
       <c r="AI8" t="s">
         <v>61</v>
@@ -1375,8 +1375,8 @@
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="17">
         <f t="shared" ref="D9:D13" si="25">W9/1000</f>
         <v>432.33263577457899</v>
@@ -1399,39 +1399,39 @@
       </c>
       <c r="I9" s="17">
         <f t="shared" si="18"/>
-        <v>2860.7262162535799</v>
+        <v>2970.9802708871898</v>
       </c>
       <c r="J9" s="19">
         <f t="shared" si="19"/>
-        <v>1.14159415425658</v>
+        <v>1.15702286643668</v>
       </c>
       <c r="K9" s="17">
         <f t="shared" si="20"/>
-        <v>379.04060474490598</v>
+        <v>393.47203395306099</v>
       </c>
       <c r="L9" s="19">
         <f t="shared" si="21"/>
-        <v>1.1552169418331499</v>
+        <v>1.16998574341338</v>
       </c>
       <c r="M9" s="20">
         <f t="shared" si="22"/>
-        <v>1.1523671089374199</v>
+        <v>1.1941161129870799</v>
       </c>
       <c r="N9" s="19">
         <f t="shared" si="23"/>
-        <v>1.2207192399678699</v>
+        <v>1.2449571203474501</v>
       </c>
       <c r="O9" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K9)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M9)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G9))</f>
-        <v>114.85972258339575</v>
+        <v>113.14465274852147</v>
       </c>
       <c r="P9" s="20">
         <f t="shared" ref="P9:P13" si="26">(K9 * 20 + M9 * 1000) /G9</f>
-        <v>148.57204559137497</v>
+        <v>154.19255021548219</v>
       </c>
       <c r="Q9" s="18">
         <f t="shared" si="24"/>
-        <v>20.547499240001919</v>
+        <v>19.784974787722494</v>
       </c>
       <c r="S9" t="s">
         <v>52</v>
@@ -1455,16 +1455,16 @@
         <v>58780.769754323999</v>
       </c>
       <c r="Z9">
-        <v>-2860.7262162535799</v>
+        <v>-2970.9802708871898</v>
       </c>
       <c r="AA9">
-        <v>-1152367.10893742</v>
+        <v>-1194116.1129870799</v>
       </c>
       <c r="AB9">
-        <v>379.04060474490598</v>
+        <v>393.47203395306099</v>
       </c>
       <c r="AC9">
-        <v>114.859722583395</v>
+        <v>113.144652748521</v>
       </c>
       <c r="AD9">
         <v>1.3337788816487699</v>
@@ -1473,13 +1473,13 @@
         <v>1.16688944082438</v>
       </c>
       <c r="AF9">
-        <v>1.14159415425658</v>
+        <v>1.15702286643668</v>
       </c>
       <c r="AG9">
-        <v>1.1552169418331499</v>
+        <v>1.16998574341338</v>
       </c>
       <c r="AH9">
-        <v>1.2207192399678699</v>
+        <v>1.2449571203474501</v>
       </c>
       <c r="AI9" t="s">
         <v>61</v>
@@ -1489,11 +1489,11 @@
       <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="27" t="str">
+      <c r="B10" s="22" t="str">
         <f>T10</f>
         <v>[85,90)</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="23">
         <f>V10/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -1519,39 +1519,39 @@
       </c>
       <c r="I10" s="17">
         <f t="shared" si="18"/>
-        <v>1881.36743124539</v>
+        <v>2013.8918608971601</v>
       </c>
       <c r="J10" s="19">
         <f t="shared" si="19"/>
-        <v>1.1711712219327399</v>
+        <v>1.18969328854939</v>
       </c>
       <c r="K10" s="17">
         <f t="shared" si="20"/>
-        <v>162.223145127067</v>
+        <v>172.28852391461299</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" si="21"/>
-        <v>1.1805334315640299</v>
+        <v>1.19762182358415</v>
       </c>
       <c r="M10" s="20">
         <f t="shared" si="22"/>
-        <v>0.55961467433486489</v>
+        <v>0.59842974890966394</v>
       </c>
       <c r="N10" s="19">
         <f t="shared" si="23"/>
-        <v>1.26170928732307</v>
+        <v>1.29045111926571</v>
       </c>
       <c r="O10" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K10)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M10)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G10))</f>
-        <v>113.79178732565737</v>
+        <v>112.2931621188512</v>
       </c>
       <c r="P10" s="20">
         <f t="shared" si="26"/>
-        <v>81.130019361215588</v>
+        <v>86.251143964039628</v>
       </c>
       <c r="Q10" s="18">
         <f t="shared" si="24"/>
-        <v>24.922646856277982</v>
+        <v>23.282608667450233</v>
       </c>
       <c r="S10" t="s">
         <v>53</v>
@@ -1575,16 +1575,16 @@
         <v>46888.656095831699</v>
       </c>
       <c r="Z10">
-        <v>-1881.36743124539</v>
+        <v>-2013.8918608971601</v>
       </c>
       <c r="AA10">
-        <v>-559614.67433486495</v>
+        <v>-598429.74890966399</v>
       </c>
       <c r="AB10">
-        <v>162.223145127067</v>
+        <v>172.28852391461299</v>
       </c>
       <c r="AC10">
-        <v>113.791787325657</v>
+        <v>112.293162118851</v>
       </c>
       <c r="AD10">
         <v>1.41008598033954</v>
@@ -1593,13 +1593,13 @@
         <v>1.2050429901697699</v>
       </c>
       <c r="AF10">
-        <v>1.1711712219327399</v>
+        <v>1.18969328854939</v>
       </c>
       <c r="AG10">
-        <v>1.1805334315640299</v>
+        <v>1.19762182358415</v>
       </c>
       <c r="AH10">
-        <v>1.26170928732307</v>
+        <v>1.29045111926571</v>
       </c>
       <c r="AI10" t="s">
         <v>61</v>
@@ -1609,8 +1609,8 @@
       <c r="A11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="17">
         <f t="shared" si="25"/>
         <v>595.70287520163299</v>
@@ -1633,39 +1633,39 @@
       </c>
       <c r="I11" s="17">
         <f t="shared" si="18"/>
-        <v>2901.69030893744</v>
+        <v>2991.2900760042098</v>
       </c>
       <c r="J11" s="19">
         <f t="shared" si="19"/>
-        <v>1.2167888345358699</v>
+        <v>1.2382195830054901</v>
       </c>
       <c r="K11" s="17">
         <f t="shared" si="20"/>
-        <v>416.07267783454301</v>
+        <v>429.17134849906301</v>
       </c>
       <c r="L11" s="19">
         <f t="shared" si="21"/>
-        <v>1.2454655944033599</v>
+        <v>1.26646340121583</v>
       </c>
       <c r="M11" s="20">
         <f t="shared" si="22"/>
-        <v>1.4645084116160199</v>
+        <v>1.50351979253798</v>
       </c>
       <c r="N11" s="19">
         <f t="shared" si="23"/>
-        <v>1.36898000751204</v>
+        <v>1.4047521344474201</v>
       </c>
       <c r="O11" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K11)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M11)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G11))</f>
-        <v>114.15648788954049</v>
+        <v>112.92827424489134</v>
       </c>
       <c r="P11" s="20">
         <f t="shared" si="26"/>
-        <v>120.82493745019346</v>
+        <v>124.54112488807085</v>
       </c>
       <c r="Q11" s="18">
         <f t="shared" si="24"/>
-        <v>27.912316781645696</v>
+        <v>27.076243710033022</v>
       </c>
       <c r="S11" t="s">
         <v>54</v>
@@ -1689,16 +1689,16 @@
         <v>80992.899105293196</v>
       </c>
       <c r="Z11">
-        <v>-2901.69030893744</v>
+        <v>-2991.2900760042098</v>
       </c>
       <c r="AA11">
-        <v>-1464508.4116160199</v>
+        <v>-1503519.79253798</v>
       </c>
       <c r="AB11">
-        <v>416.07267783454301</v>
+        <v>429.17134849906301</v>
       </c>
       <c r="AC11">
-        <v>114.15648788954</v>
+        <v>112.928274244891</v>
       </c>
       <c r="AD11">
         <v>1.5418946876023101</v>
@@ -1707,13 +1707,13 @@
         <v>1.27094734380115</v>
       </c>
       <c r="AF11">
-        <v>1.2167888345358699</v>
+        <v>1.2382195830054901</v>
       </c>
       <c r="AG11">
-        <v>1.2454655944033599</v>
+        <v>1.26646340121583</v>
       </c>
       <c r="AH11">
-        <v>1.36898000751204</v>
+        <v>1.4047521344474201</v>
       </c>
       <c r="AI11" t="s">
         <v>61</v>
@@ -1753,39 +1753,39 @@
       </c>
       <c r="I12" s="17">
         <f t="shared" si="18"/>
-        <v>1436.4970518170301</v>
+        <v>1477.3691476014601</v>
       </c>
       <c r="J12" s="19">
         <f t="shared" si="19"/>
-        <v>1.2393720736270599</v>
+        <v>1.2621862490443201</v>
       </c>
       <c r="K12" s="17">
         <f t="shared" si="20"/>
-        <v>217.099695009676</v>
+        <v>222.88904099605199</v>
       </c>
       <c r="L12" s="19">
         <f t="shared" si="21"/>
-        <v>1.2793461001412101</v>
+        <v>1.30221609829741</v>
       </c>
       <c r="M12" s="20">
         <f t="shared" si="22"/>
-        <v>0.85629839067426894</v>
+        <v>0.87716270430148302</v>
       </c>
       <c r="N12" s="19">
         <f t="shared" si="23"/>
-        <v>1.4317012212215099</v>
+        <v>1.47143605046821</v>
       </c>
       <c r="O12" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K12)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M12)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G12))</f>
-        <v>113.36812329198703</v>
+        <v>112.26736796704174</v>
       </c>
       <c r="P12" s="20">
         <f t="shared" si="26"/>
-        <v>91.656589339778492</v>
+        <v>94.066031763855449</v>
       </c>
       <c r="Q12" s="18">
         <f t="shared" si="24"/>
-        <v>39.481374515680592</v>
+        <v>38.389104162312442</v>
       </c>
       <c r="S12" t="s">
         <v>54</v>
@@ -1809,16 +1809,16 @@
         <v>56714.8780934592</v>
       </c>
       <c r="Z12">
-        <v>-1436.4970518170301</v>
+        <v>-1477.3691476014601</v>
       </c>
       <c r="AA12">
-        <v>-856298.39067426894</v>
+        <v>-877162.704301483</v>
       </c>
       <c r="AB12">
-        <v>217.099695009676</v>
+        <v>222.88904099605199</v>
       </c>
       <c r="AC12">
-        <v>113.368123291986</v>
+        <v>112.267367967041</v>
       </c>
       <c r="AD12">
         <v>1.63419308470433</v>
@@ -1827,13 +1827,13 @@
         <v>1.3170965423521599</v>
       </c>
       <c r="AF12">
-        <v>1.2393720736270599</v>
+        <v>1.2621862490443201</v>
       </c>
       <c r="AG12">
-        <v>1.2793461001412101</v>
+        <v>1.30221609829741</v>
       </c>
       <c r="AH12">
-        <v>1.4317012212215099</v>
+        <v>1.47143605046821</v>
       </c>
       <c r="AI12" t="s">
         <v>61</v>
@@ -1873,39 +1873,39 @@
       </c>
       <c r="I13" s="17">
         <f t="shared" si="18"/>
-        <v>236.73542760277701</v>
+        <v>242.50151599851301</v>
       </c>
       <c r="J13" s="19">
         <f t="shared" si="19"/>
-        <v>1.2430938026456799</v>
+        <v>1.2661202372809599</v>
       </c>
       <c r="K13" s="17">
         <f t="shared" si="20"/>
-        <v>34.789645891475402</v>
+        <v>35.483222543958902</v>
       </c>
       <c r="L13" s="19">
         <f t="shared" si="21"/>
-        <v>1.28477536063461</v>
+        <v>1.3079078133383299</v>
       </c>
       <c r="M13" s="20">
         <f t="shared" si="22"/>
-        <v>0.14453224208097099</v>
+        <v>0.147012741783423</v>
       </c>
       <c r="N13" s="19">
         <f t="shared" si="23"/>
-        <v>1.4422877617805001</v>
+        <v>1.4826122955126</v>
       </c>
       <c r="O13" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$8:K13)) * 20 + (SUM($M$3:$M$5) + SUM($M$8:M13)) * 1000) /(SUM($G$3:$G$5) + SUM($G$8:G13))</f>
-        <v>112.85341530025873</v>
+        <v>111.77266319120876</v>
       </c>
       <c r="P13" s="20">
         <f t="shared" si="26"/>
-        <v>56.669410734518557</v>
+        <v>57.772150607823107</v>
       </c>
       <c r="Q13" s="18">
         <f t="shared" si="24"/>
-        <v>62.637644097176327</v>
+        <v>61.148275293530645</v>
       </c>
       <c r="S13" t="s">
         <v>55</v>
@@ -1929,16 +1929,16 @@
         <v>14828.549459375599</v>
       </c>
       <c r="Z13">
-        <v>-236.73542760277701</v>
+        <v>-242.50151599851301</v>
       </c>
       <c r="AA13">
-        <v>-144532.24208097099</v>
+        <v>-147012.741783423</v>
       </c>
       <c r="AB13">
-        <v>34.789645891475402</v>
+        <v>35.483222543958902</v>
       </c>
       <c r="AC13">
-        <v>112.85341530025801</v>
+        <v>111.772663191208</v>
       </c>
       <c r="AD13">
         <v>1.65832522414388</v>
@@ -1947,13 +1947,13 @@
         <v>1.32916261207194</v>
       </c>
       <c r="AF13">
-        <v>1.2430938026456799</v>
+        <v>1.2661202372809599</v>
       </c>
       <c r="AG13">
-        <v>1.28477536063461</v>
+        <v>1.3079078133383299</v>
       </c>
       <c r="AH13">
-        <v>1.4422877617805001</v>
+        <v>1.4826122955126</v>
       </c>
       <c r="AI13" t="s">
         <v>61</v>
@@ -1979,23 +1979,23 @@
       <c r="Q14" s="18"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="18"/>
     </row>
@@ -2003,10 +2003,10 @@
       <c r="A16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="23">
         <v>1508.4970000000001</v>
       </c>
       <c r="D16" s="17">
@@ -2031,39 +2031,39 @@
       </c>
       <c r="I16" s="17">
         <f t="shared" ref="I16:I21" si="32">-Z16</f>
-        <v>8089.1455318831604</v>
+        <v>8227.6866740854493</v>
       </c>
       <c r="J16" s="19">
         <f t="shared" ref="J16:J21" si="33">AF16</f>
-        <v>1.1271698451165499</v>
+        <v>1.13347389791513</v>
       </c>
       <c r="K16" s="17">
         <f t="shared" ref="K16:K21" si="34">AB16</f>
-        <v>811.65090162591696</v>
+        <v>819.70537271405999</v>
       </c>
       <c r="L16" s="19">
         <f t="shared" ref="L16:L21" si="35">AG16</f>
-        <v>1.1266659680403699</v>
+        <v>1.1314855039791301</v>
       </c>
       <c r="M16" s="20">
         <f t="shared" ref="M16:M21" si="36">-AA16/1000000</f>
-        <v>2.4606020896132899</v>
+        <v>2.48039997451226</v>
       </c>
       <c r="N16" s="19">
         <f t="shared" ref="N16:N21" si="37">AH16</f>
-        <v>1.18023150714447</v>
+        <v>1.1885656820419099</v>
       </c>
       <c r="O16" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K16)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M16)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G16))</f>
-        <v>105.4838374579991</v>
+        <v>102.99308764053391</v>
       </c>
       <c r="P16" s="20">
         <f>(K16 * 20 + M16 * 1000) /G16</f>
-        <v>63.880390475738757</v>
+        <v>64.498523919457455</v>
       </c>
       <c r="Q16" s="18">
         <f t="shared" ref="Q16:Q21" si="38">E16/I16*1000</f>
-        <v>18.088110662312214</v>
+        <v>17.783535681433193</v>
       </c>
       <c r="S16" t="s">
         <v>51</v>
@@ -2087,16 +2087,16 @@
         <v>292634.719088502</v>
       </c>
       <c r="Z16">
-        <v>-8089.1455318831604</v>
+        <v>-8227.6866740854493</v>
       </c>
       <c r="AA16">
-        <v>-2460602.08961329</v>
+        <v>-2480399.9745122599</v>
       </c>
       <c r="AB16">
-        <v>811.65090162591696</v>
+        <v>819.70537271405999</v>
       </c>
       <c r="AC16">
-        <v>105.483837457999</v>
+        <v>102.99308764053301</v>
       </c>
       <c r="AD16">
         <v>1.2381184304386501</v>
@@ -2105,13 +2105,13 @@
         <v>1.2381184304386501</v>
       </c>
       <c r="AF16">
-        <v>1.1271698451165499</v>
+        <v>1.13347389791513</v>
       </c>
       <c r="AG16">
-        <v>1.1266659680403699</v>
+        <v>1.1314855039791301</v>
       </c>
       <c r="AH16">
-        <v>1.18023150714447</v>
+        <v>1.1885656820419099</v>
       </c>
       <c r="AI16" t="s">
         <v>62</v>
@@ -2121,8 +2121,8 @@
       <c r="A17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="17">
         <f t="shared" si="27"/>
         <v>432.33263577457899</v>
@@ -2145,39 +2145,39 @@
       </c>
       <c r="I17" s="17">
         <f t="shared" si="32"/>
-        <v>3430.6079983241498</v>
+        <v>3401.68027509177</v>
       </c>
       <c r="J17" s="19">
         <f t="shared" si="33"/>
-        <v>1.1811025980980601</v>
+        <v>1.18865775988786</v>
       </c>
       <c r="K17" s="17">
         <f t="shared" si="34"/>
-        <v>454.21820070532499</v>
+        <v>450.01264339643399</v>
       </c>
       <c r="L17" s="19">
         <f t="shared" si="35"/>
-        <v>1.19755110841124</v>
+        <v>1.2036701463928401</v>
       </c>
       <c r="M17" s="20">
         <f t="shared" si="36"/>
-        <v>1.3848462257213801</v>
+        <v>1.36683611281877</v>
       </c>
       <c r="N17" s="19">
         <f t="shared" si="37"/>
-        <v>1.2816672181351501</v>
+        <v>1.2924756911136801</v>
       </c>
       <c r="O17" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K17)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M17)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G17))</f>
-        <v>104.30539675594223</v>
+        <v>101.93098529169602</v>
       </c>
       <c r="P17" s="20">
         <f t="shared" ref="P17:P21" si="39">(K17 * 20 + M17 * 1000) /G17</f>
-        <v>89.053020941919101</v>
+        <v>88.184358796907659</v>
       </c>
       <c r="Q17" s="18">
         <f t="shared" si="38"/>
-        <v>17.134213463921956</v>
+        <v>17.279921979950988</v>
       </c>
       <c r="S17" t="s">
         <v>52</v>
@@ -2201,16 +2201,16 @@
         <v>117561.539508648</v>
       </c>
       <c r="Z17">
-        <v>-3430.6079983241498</v>
+        <v>-3401.68027509177</v>
       </c>
       <c r="AA17">
-        <v>-1384846.22572138</v>
+        <v>-1366836.1128187701</v>
       </c>
       <c r="AB17">
-        <v>454.21820070532499</v>
+        <v>450.01264339643399</v>
       </c>
       <c r="AC17">
-        <v>104.305396755942</v>
+        <v>101.930985291696</v>
       </c>
       <c r="AD17">
         <v>1.3337788816487699</v>
@@ -2219,13 +2219,13 @@
         <v>1.3337788816487699</v>
       </c>
       <c r="AF17">
-        <v>1.1811025980980601</v>
+        <v>1.18865775988786</v>
       </c>
       <c r="AG17">
-        <v>1.19755110841124</v>
+        <v>1.2036701463928401</v>
       </c>
       <c r="AH17">
-        <v>1.2816672181351501</v>
+        <v>1.2924756911136801</v>
       </c>
       <c r="AI17" t="s">
         <v>62</v>
@@ -2235,11 +2235,11 @@
       <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="27" t="str">
+      <c r="B18" s="22" t="str">
         <f>T18</f>
         <v>[85,90)</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="23">
         <v>940.56899999999996</v>
       </c>
       <c r="D18" s="17">
@@ -2264,39 +2264,39 @@
       </c>
       <c r="I18" s="17">
         <f t="shared" si="32"/>
-        <v>2418.0540310684501</v>
+        <v>2446.1601279562801</v>
       </c>
       <c r="J18" s="19">
         <f t="shared" si="33"/>
-        <v>1.2191169415664</v>
+        <v>1.2283406671418799</v>
       </c>
       <c r="K18" s="17">
         <f t="shared" si="34"/>
-        <v>208.27752535254399</v>
+        <v>210.052717532841</v>
       </c>
       <c r="L18" s="19">
         <f t="shared" si="35"/>
-        <v>1.23005482930526</v>
+        <v>1.2373638226164601</v>
       </c>
       <c r="M18" s="20">
         <f t="shared" si="36"/>
-        <v>0.72091459386456902</v>
+        <v>0.72697001475812495</v>
       </c>
       <c r="N18" s="19">
         <f t="shared" si="37"/>
-        <v>1.3344719866603501</v>
+        <v>1.34774161518459</v>
       </c>
       <c r="O18" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K18)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M18)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G18))</f>
-        <v>101.48067573461189</v>
+        <v>99.258738266940654</v>
       </c>
       <c r="P18" s="20">
         <f t="shared" si="39"/>
-        <v>52.107114041916844</v>
+        <v>52.550283754592733</v>
       </c>
       <c r="Q18" s="18">
         <f t="shared" si="38"/>
-        <v>19.391070461363224</v>
+        <v>19.168269305005097</v>
       </c>
       <c r="S18" t="s">
         <v>53</v>
@@ -2320,16 +2320,16 @@
         <v>93777.312191663499</v>
       </c>
       <c r="Z18">
-        <v>-2418.0540310684501</v>
+        <v>-2446.1601279562801</v>
       </c>
       <c r="AA18">
-        <v>-720914.59386456897</v>
+        <v>-726970.01475812495</v>
       </c>
       <c r="AB18">
-        <v>208.27752535254399</v>
+        <v>210.052717532841</v>
       </c>
       <c r="AC18">
-        <v>101.480675734611</v>
+        <v>99.258738266940696</v>
       </c>
       <c r="AD18">
         <v>1.41008598033954</v>
@@ -2338,13 +2338,13 @@
         <v>1.41008598033954</v>
       </c>
       <c r="AF18">
-        <v>1.2191169415664</v>
+        <v>1.2283406671418799</v>
       </c>
       <c r="AG18">
-        <v>1.23005482930526</v>
+        <v>1.2373638226164601</v>
       </c>
       <c r="AH18">
-        <v>1.3344719866603501</v>
+        <v>1.34774161518459</v>
       </c>
       <c r="AI18" t="s">
         <v>62</v>
@@ -2354,8 +2354,8 @@
       <c r="A19" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="17">
         <f t="shared" si="27"/>
         <v>595.70287520163299</v>
@@ -2378,39 +2378,39 @@
       </c>
       <c r="I19" s="17">
         <f t="shared" si="32"/>
-        <v>3441.1441042000301</v>
+        <v>3421.9017297001901</v>
       </c>
       <c r="J19" s="19">
         <f t="shared" si="33"/>
-        <v>1.2732153331740299</v>
+        <v>1.2838525722784999</v>
       </c>
       <c r="K19" s="17">
         <f t="shared" si="34"/>
-        <v>492.49389436391402</v>
+        <v>489.89476123665298</v>
       </c>
       <c r="L19" s="19">
         <f t="shared" si="35"/>
-        <v>1.3069132616172501</v>
+        <v>1.31594578843262</v>
       </c>
       <c r="M19" s="20">
         <f t="shared" si="36"/>
-        <v>1.7376057270065899</v>
+        <v>1.71789924427458</v>
       </c>
       <c r="N19" s="19">
         <f t="shared" si="37"/>
-        <v>1.4617462421457199</v>
+        <v>1.4783402468587501</v>
       </c>
       <c r="O19" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K19)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M19)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G19))</f>
-        <v>98.92068279656317</v>
+        <v>96.850854852038054</v>
       </c>
       <c r="P19" s="20">
         <f t="shared" si="39"/>
-        <v>71.533947681146856</v>
+        <v>71.091383295446619</v>
       </c>
       <c r="Q19" s="18">
         <f t="shared" si="38"/>
-        <v>23.536619407027647</v>
+        <v>23.668972841131058</v>
       </c>
       <c r="S19" t="s">
         <v>54</v>
@@ -2434,16 +2434,16 @@
         <v>161985.79821058601</v>
       </c>
       <c r="Z19">
-        <v>-3441.1441042000301</v>
+        <v>-3421.9017297001901</v>
       </c>
       <c r="AA19">
-        <v>-1737605.72700659</v>
+        <v>-1717899.2442745799</v>
       </c>
       <c r="AB19">
-        <v>492.49389436391402</v>
+        <v>489.89476123665298</v>
       </c>
       <c r="AC19">
-        <v>98.920682796563099</v>
+        <v>96.850854852037997</v>
       </c>
       <c r="AD19">
         <v>1.5418946876023101</v>
@@ -2452,13 +2452,13 @@
         <v>1.5418946876023101</v>
       </c>
       <c r="AF19">
-        <v>1.2732153331740299</v>
+        <v>1.2838525722784999</v>
       </c>
       <c r="AG19">
-        <v>1.3069132616172501</v>
+        <v>1.31594578843262</v>
       </c>
       <c r="AH19">
-        <v>1.4617462421457199</v>
+        <v>1.4783402468587501</v>
       </c>
       <c r="AI19" t="s">
         <v>62</v>
@@ -2497,39 +2497,39 @@
       </c>
       <c r="I20" s="17">
         <f t="shared" si="32"/>
-        <v>1689.26682976081</v>
+        <v>1687.40184965618</v>
       </c>
       <c r="J20" s="19">
         <f t="shared" si="33"/>
-        <v>1.2997723780750601</v>
+        <v>1.31122650022987</v>
       </c>
       <c r="K20" s="17">
         <f t="shared" si="34"/>
-        <v>254.78764804356101</v>
+        <v>254.776716327858</v>
       </c>
       <c r="L20" s="19">
         <f t="shared" si="35"/>
-        <v>1.34667533669105</v>
+        <v>1.35681345389344</v>
       </c>
       <c r="M20" s="20">
         <f t="shared" si="36"/>
-        <v>1.0054838530916901</v>
+        <v>1.0028080909625301</v>
       </c>
       <c r="N20" s="19">
         <f t="shared" si="37"/>
-        <v>1.53539483043925</v>
+        <v>1.5545760126919099</v>
       </c>
       <c r="O20" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K20)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M20)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G20))</f>
-        <v>96.371650132698591</v>
+        <v>94.417283829464196</v>
       </c>
       <c r="P20" s="20">
         <f t="shared" si="39"/>
-        <v>53.788679611625348</v>
+        <v>53.763162529154933</v>
       </c>
       <c r="Q20" s="18">
         <f t="shared" si="38"/>
-        <v>33.573664677645795</v>
+        <v>33.610771556885069</v>
       </c>
       <c r="S20" t="s">
         <v>54</v>
@@ -2553,16 +2553,16 @@
         <v>113429.75618691801</v>
       </c>
       <c r="Z20">
-        <v>-1689.26682976081</v>
+        <v>-1687.40184965618</v>
       </c>
       <c r="AA20">
-        <v>-1005483.85309169</v>
+        <v>-1002808.09096253</v>
       </c>
       <c r="AB20">
-        <v>254.78764804356101</v>
+        <v>254.776716327858</v>
       </c>
       <c r="AC20">
-        <v>96.371650132698505</v>
+        <v>94.417283829464196</v>
       </c>
       <c r="AD20">
         <v>1.63419308470433</v>
@@ -2571,13 +2571,13 @@
         <v>1.63419308470433</v>
       </c>
       <c r="AF20">
-        <v>1.2997723780750601</v>
+        <v>1.31122650022987</v>
       </c>
       <c r="AG20">
-        <v>1.34667533669105</v>
+        <v>1.35681345389344</v>
       </c>
       <c r="AH20">
-        <v>1.53539483043925</v>
+        <v>1.5545760126919099</v>
       </c>
       <c r="AI20" t="s">
         <v>62</v>
@@ -2616,39 +2616,39 @@
       </c>
       <c r="I21" s="17">
         <f t="shared" si="32"/>
-        <v>275.50396614288502</v>
+        <v>277.23480019250798</v>
       </c>
       <c r="J21" s="19">
         <f t="shared" si="33"/>
-        <v>1.3041035891486299</v>
+        <v>1.31572395022829</v>
       </c>
       <c r="K21" s="17">
         <f t="shared" si="34"/>
-        <v>40.389101170818698</v>
+        <v>40.5672077956918</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="35"/>
-        <v>1.3529784463011401</v>
+        <v>1.3633206697048801</v>
       </c>
       <c r="M21" s="20">
         <f t="shared" si="36"/>
-        <v>0.167633713289075</v>
+        <v>0.16826237552079701</v>
       </c>
       <c r="N21" s="19">
         <f t="shared" si="37"/>
-        <v>1.5476734824496099</v>
+        <v>1.5673677035192299</v>
       </c>
       <c r="O21" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$16:K21)) * 20 + (SUM($M$3:$M$5) + SUM($M$16:M21)) * 1000) /(SUM($G$3:$G$5) + SUM($G$16:G21))</f>
-        <v>95.447854791742373</v>
+        <v>93.523984986670172</v>
       </c>
       <c r="P21" s="20">
         <f t="shared" si="39"/>
-        <v>32.889789368059951</v>
+        <v>33.03109768485335</v>
       </c>
       <c r="Q21" s="18">
         <f t="shared" si="38"/>
-        <v>53.823361118819783</v>
+        <v>53.487330771890328</v>
       </c>
       <c r="S21" t="s">
         <v>55</v>
@@ -2672,16 +2672,16 @@
         <v>29657.098918751301</v>
       </c>
       <c r="Z21">
-        <v>-275.50396614288502</v>
+        <v>-277.23480019250798</v>
       </c>
       <c r="AA21">
-        <v>-167633.71328907501</v>
+        <v>-168262.37552079701</v>
       </c>
       <c r="AB21">
-        <v>40.389101170818698</v>
+        <v>40.5672077956918</v>
       </c>
       <c r="AC21">
-        <v>95.447854791742301</v>
+        <v>93.523984986670101</v>
       </c>
       <c r="AD21">
         <v>1.65832522414388</v>
@@ -2690,13 +2690,13 @@
         <v>1.65832522414388</v>
       </c>
       <c r="AF21">
-        <v>1.3041035891486299</v>
+        <v>1.31572395022829</v>
       </c>
       <c r="AG21">
-        <v>1.3529784463011401</v>
+        <v>1.3633206697048801</v>
       </c>
       <c r="AH21">
-        <v>1.5476734824496099</v>
+        <v>1.5673677035192299</v>
       </c>
       <c r="AI21" t="s">
         <v>62</v>
@@ -2725,23 +2725,23 @@
       <c r="Q22" s="14"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
       <c r="P23" s="20"/>
       <c r="Q23" s="18"/>
     </row>
@@ -2749,11 +2749,11 @@
       <c r="A24" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="27" t="str">
+      <c r="B24" s="22" t="str">
         <f>T24</f>
         <v>[80,85)</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="23">
         <f>V24/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -2779,39 +2779,39 @@
       </c>
       <c r="I24" s="17">
         <f t="shared" ref="I24:I29" si="44">-Z24</f>
-        <v>11202.7804956871</v>
+        <v>12253.3163549091</v>
       </c>
       <c r="J24" s="19">
         <f t="shared" ref="J24:J29" si="45">AF24</f>
-        <v>1.17611944981037</v>
+        <v>1.1987797981452399</v>
       </c>
       <c r="K24" s="17">
         <f t="shared" ref="K24:K29" si="46">AB24</f>
-        <v>1125.9799341390001</v>
+        <v>1220.2889671560499</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" ref="L24:L29" si="47">AG24</f>
-        <v>1.17572005164541</v>
+        <v>1.1957414397754</v>
       </c>
       <c r="M24" s="20">
         <f t="shared" ref="M24:M29" si="48">-AA24/1000000</f>
-        <v>3.3293928103482098</v>
+        <v>3.6361200818484201</v>
       </c>
       <c r="N24" s="19">
         <f t="shared" ref="N24:N29" si="49">AH24</f>
-        <v>1.2438677454668501</v>
+        <v>1.2764261692733001</v>
       </c>
       <c r="O24" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K24)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M24)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G24))</f>
-        <v>112.84882090500037</v>
+        <v>111.65216135811444</v>
       </c>
       <c r="P24" s="20">
         <f>(K24 * 20 + M24 * 1000) /G24</f>
-        <v>100.68287444985334</v>
+        <v>109.22434014070443</v>
       </c>
       <c r="Q24" s="18">
         <f t="shared" ref="Q24:Q29" si="50">E24/I24*1000</f>
-        <v>22.917232514621769</v>
+        <v>20.952427734151609</v>
       </c>
       <c r="S24" t="s">
         <v>51</v>
@@ -2835,16 +2835,16 @@
         <v>256736.72542993099</v>
       </c>
       <c r="Z24">
-        <v>-11202.7804956871</v>
+        <v>-12253.3163549091</v>
       </c>
       <c r="AA24">
-        <v>-3329392.8103482099</v>
+        <v>-3636120.0818484202</v>
       </c>
       <c r="AB24">
-        <v>1125.9799341390001</v>
+        <v>1220.2889671560499</v>
       </c>
       <c r="AC24">
-        <v>112.848820905</v>
+        <v>111.652161358114</v>
       </c>
       <c r="AD24">
         <v>1.4178160833803599</v>
@@ -2853,13 +2853,13 @@
         <v>1.2089080416901801</v>
       </c>
       <c r="AF24">
-        <v>1.17611944981037</v>
+        <v>1.1987797981452399</v>
       </c>
       <c r="AG24">
-        <v>1.17572005164541</v>
+        <v>1.1957414397754</v>
       </c>
       <c r="AH24">
-        <v>1.2438677454668501</v>
+        <v>1.2764261692733001</v>
       </c>
       <c r="AI24" t="s">
         <v>63</v>
@@ -2869,8 +2869,8 @@
       <c r="A25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="17">
         <f t="shared" ref="D25:D29" si="51">W25/1000</f>
         <v>432.33263577457899</v>
@@ -2893,39 +2893,39 @@
       </c>
       <c r="I25" s="17">
         <f t="shared" si="44"/>
-        <v>3849.1837942556799</v>
+        <v>4000.1614705817601</v>
       </c>
       <c r="J25" s="19">
         <f t="shared" si="45"/>
-        <v>1.23663265296778</v>
+        <v>1.26367253955823</v>
       </c>
       <c r="K25" s="17">
         <f t="shared" si="46"/>
-        <v>504.84752937841398</v>
+        <v>524.266627907724</v>
       </c>
       <c r="L25" s="19">
         <f t="shared" si="47"/>
-        <v>1.25450638810287</v>
+        <v>1.2798368526938899</v>
       </c>
       <c r="M25" s="20">
         <f t="shared" si="48"/>
-        <v>1.5078813828092001</v>
+        <v>1.5644777091581601</v>
       </c>
       <c r="N25" s="19">
         <f t="shared" si="49"/>
-        <v>1.35431540190264</v>
+        <v>1.3953613447684501</v>
       </c>
       <c r="O25" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K25)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M25)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G25))</f>
-        <v>114.74143721719051</v>
+        <v>113.8882946933541</v>
       </c>
       <c r="P25" s="20">
         <f t="shared" ref="P25:P29" si="52">(K25 * 20 + M25 * 1000) /G25</f>
-        <v>151.4334621607733</v>
+        <v>157.24006102091207</v>
       </c>
       <c r="Q25" s="18">
         <f t="shared" si="50"/>
-        <v>19.908950020214487</v>
+        <v>19.157528600291929</v>
       </c>
       <c r="S25" t="s">
         <v>52</v>
@@ -2949,16 +2949,16 @@
         <v>76633.207778455893</v>
       </c>
       <c r="Z25">
-        <v>-3849.1837942556799</v>
+        <v>-4000.1614705817601</v>
       </c>
       <c r="AA25">
-        <v>-1507881.3828092001</v>
+        <v>-1564477.70915816</v>
       </c>
       <c r="AB25">
-        <v>504.84752937841398</v>
+        <v>524.266627907724</v>
       </c>
       <c r="AC25">
-        <v>114.74143721719</v>
+        <v>113.888294693354</v>
       </c>
       <c r="AD25">
         <v>1.54252978251027</v>
@@ -2967,13 +2967,13 @@
         <v>1.2712648912551301</v>
       </c>
       <c r="AF25">
-        <v>1.23663265296778</v>
+        <v>1.26367253955823</v>
       </c>
       <c r="AG25">
-        <v>1.25450638810287</v>
+        <v>1.2798368526938899</v>
       </c>
       <c r="AH25">
-        <v>1.35431540190264</v>
+        <v>1.3953613447684501</v>
       </c>
       <c r="AI25" t="s">
         <v>63</v>
@@ -2983,11 +2983,11 @@
       <c r="A26" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="27" t="str">
+      <c r="B26" s="22" t="str">
         <f>T26</f>
         <v>[85,90)</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="23">
         <f>V26/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -3013,39 +3013,39 @@
       </c>
       <c r="I26" s="17">
         <f t="shared" si="44"/>
-        <v>1881.36743124539</v>
+        <v>2013.8918608971601</v>
       </c>
       <c r="J26" s="19">
         <f t="shared" si="45"/>
-        <v>1.26620972064394</v>
+        <v>1.2963429616709401</v>
       </c>
       <c r="K26" s="17">
         <f t="shared" si="46"/>
-        <v>162.223145127067</v>
+        <v>172.28852391461299</v>
       </c>
       <c r="L26" s="19">
         <f t="shared" si="47"/>
-        <v>1.2798228778337599</v>
+        <v>1.3074729328646499</v>
       </c>
       <c r="M26" s="20">
         <f t="shared" si="48"/>
-        <v>0.55961467433486489</v>
+        <v>0.59842974890966394</v>
       </c>
       <c r="N26" s="19">
         <f t="shared" si="49"/>
-        <v>1.3953054492578301</v>
+        <v>1.44085534368671</v>
       </c>
       <c r="O26" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K26)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M26)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G26))</f>
-        <v>113.76207504389751</v>
+        <v>113.08300941446858</v>
       </c>
       <c r="P26" s="20">
         <f t="shared" si="52"/>
-        <v>81.130019361215588</v>
+        <v>86.251143964039628</v>
       </c>
       <c r="Q26" s="18">
         <f t="shared" si="50"/>
-        <v>24.922646856277982</v>
+        <v>23.282608667450233</v>
       </c>
       <c r="S26" t="s">
         <v>53</v>
@@ -3069,16 +3069,16 @@
         <v>46888.656095831699</v>
       </c>
       <c r="Z26">
-        <v>-1881.36743124539</v>
+        <v>-2013.8918608971601</v>
       </c>
       <c r="AA26">
-        <v>-559614.67433486495</v>
+        <v>-598429.74890966399</v>
       </c>
       <c r="AB26">
-        <v>162.223145127067</v>
+        <v>172.28852391461299</v>
       </c>
       <c r="AC26">
-        <v>113.762075043897</v>
+        <v>113.08300941446799</v>
       </c>
       <c r="AD26">
         <v>1.6188368812010501</v>
@@ -3087,13 +3087,13 @@
         <v>1.30941844060052</v>
       </c>
       <c r="AF26">
-        <v>1.26620972064394</v>
+        <v>1.2963429616709401</v>
       </c>
       <c r="AG26">
-        <v>1.2798228778337599</v>
+        <v>1.3074729328646499</v>
       </c>
       <c r="AH26">
-        <v>1.3953054492578301</v>
+        <v>1.44085534368671</v>
       </c>
       <c r="AI26" t="s">
         <v>63</v>
@@ -3103,8 +3103,8 @@
       <c r="A27" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="28"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="17">
         <f t="shared" si="51"/>
         <v>595.70287520163299</v>
@@ -3127,39 +3127,39 @@
       </c>
       <c r="I27" s="17">
         <f t="shared" si="44"/>
-        <v>2901.69030893744</v>
+        <v>2991.2900760042098</v>
       </c>
       <c r="J27" s="19">
         <f t="shared" si="45"/>
-        <v>1.31182733324707</v>
+        <v>1.3448692561270399</v>
       </c>
       <c r="K27" s="17">
         <f t="shared" si="46"/>
-        <v>416.07267783454301</v>
+        <v>429.17134849906301</v>
       </c>
       <c r="L27" s="19">
         <f t="shared" si="47"/>
-        <v>1.3447550406730799</v>
+        <v>1.3763145104963399</v>
       </c>
       <c r="M27" s="20">
         <f t="shared" si="48"/>
-        <v>1.4645084116160199</v>
+        <v>1.50351979253798</v>
       </c>
       <c r="N27" s="19">
         <f t="shared" si="49"/>
-        <v>1.5025761694468001</v>
+        <v>1.5551563588684201</v>
       </c>
       <c r="O27" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K27)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M27)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G27))</f>
-        <v>114.10052168611601</v>
+        <v>113.63207302141855</v>
       </c>
       <c r="P27" s="20">
         <f t="shared" si="52"/>
-        <v>120.82493745019346</v>
+        <v>124.54112488807085</v>
       </c>
       <c r="Q27" s="18">
         <f t="shared" si="50"/>
-        <v>27.912316781645696</v>
+        <v>27.076243710033022</v>
       </c>
       <c r="S27" t="s">
         <v>54</v>
@@ -3183,16 +3183,16 @@
         <v>80992.899105293196</v>
       </c>
       <c r="Z27">
-        <v>-2901.69030893744</v>
+        <v>-2991.2900760042098</v>
       </c>
       <c r="AA27">
-        <v>-1464508.4116160199</v>
+        <v>-1503519.79253798</v>
       </c>
       <c r="AB27">
-        <v>416.07267783454301</v>
+        <v>429.17134849906301</v>
       </c>
       <c r="AC27">
-        <v>114.100521686116</v>
+        <v>113.63207302141799</v>
       </c>
       <c r="AD27">
         <v>1.7506455884638199</v>
@@ -3201,13 +3201,13 @@
         <v>1.37532279423191</v>
       </c>
       <c r="AF27">
-        <v>1.31182733324707</v>
+        <v>1.3448692561270399</v>
       </c>
       <c r="AG27">
-        <v>1.3447550406730799</v>
+        <v>1.3763145104963399</v>
       </c>
       <c r="AH27">
-        <v>1.5025761694468001</v>
+        <v>1.5551563588684201</v>
       </c>
       <c r="AI27" t="s">
         <v>63</v>
@@ -3247,39 +3247,39 @@
       </c>
       <c r="I28" s="17">
         <f t="shared" si="44"/>
-        <v>1436.4970518170301</v>
+        <v>1477.3691476014601</v>
       </c>
       <c r="J28" s="19">
         <f t="shared" si="45"/>
-        <v>1.33441057233826</v>
+        <v>1.3688359221658699</v>
       </c>
       <c r="K28" s="17">
         <f t="shared" si="46"/>
-        <v>217.099695009676</v>
+        <v>222.88904099605199</v>
       </c>
       <c r="L28" s="19">
         <f t="shared" si="47"/>
-        <v>1.3786355464109401</v>
+        <v>1.4120672075779199</v>
       </c>
       <c r="M28" s="20">
         <f t="shared" si="48"/>
-        <v>0.85629839067426894</v>
+        <v>0.87716270430148302</v>
       </c>
       <c r="N28" s="19">
         <f t="shared" si="49"/>
-        <v>1.56529738315627</v>
+        <v>1.62184027488921</v>
       </c>
       <c r="O28" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K28)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M28)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G28))</f>
-        <v>113.3718618916386</v>
+        <v>112.99684620904588</v>
       </c>
       <c r="P28" s="20">
         <f t="shared" si="52"/>
-        <v>91.656589339778492</v>
+        <v>94.066031763855449</v>
       </c>
       <c r="Q28" s="18">
         <f t="shared" si="50"/>
-        <v>39.481374515680592</v>
+        <v>38.389104162312442</v>
       </c>
       <c r="S28" t="s">
         <v>54</v>
@@ -3303,16 +3303,16 @@
         <v>56714.8780934592</v>
       </c>
       <c r="Z28">
-        <v>-1436.4970518170301</v>
+        <v>-1477.3691476014601</v>
       </c>
       <c r="AA28">
-        <v>-856298.39067426894</v>
+        <v>-877162.704301483</v>
       </c>
       <c r="AB28">
-        <v>217.099695009676</v>
+        <v>222.88904099605199</v>
       </c>
       <c r="AC28">
-        <v>113.37186189163801</v>
+        <v>112.996846209046</v>
       </c>
       <c r="AD28">
         <v>1.8429439855658301</v>
@@ -3321,13 +3321,13 @@
         <v>1.42147199278291</v>
       </c>
       <c r="AF28">
-        <v>1.33441057233826</v>
+        <v>1.3688359221658699</v>
       </c>
       <c r="AG28">
-        <v>1.3786355464109401</v>
+        <v>1.4120672075779199</v>
       </c>
       <c r="AH28">
-        <v>1.56529738315627</v>
+        <v>1.62184027488921</v>
       </c>
       <c r="AI28" t="s">
         <v>63</v>
@@ -3367,39 +3367,39 @@
       </c>
       <c r="I29" s="17">
         <f t="shared" si="44"/>
-        <v>236.73542760277701</v>
+        <v>242.50151599851301</v>
       </c>
       <c r="J29" s="19">
         <f t="shared" si="45"/>
-        <v>1.33813230135688</v>
+        <v>1.37276991040251</v>
       </c>
       <c r="K29" s="17">
         <f t="shared" si="46"/>
-        <v>34.789645891475402</v>
+        <v>35.483222543958902</v>
       </c>
       <c r="L29" s="19">
         <f t="shared" si="47"/>
-        <v>1.38406480690433</v>
+        <v>1.4177589226188301</v>
       </c>
       <c r="M29" s="20">
         <f t="shared" si="48"/>
-        <v>0.14453224208097099</v>
+        <v>0.147012741783423</v>
       </c>
       <c r="N29" s="19">
         <f t="shared" si="49"/>
-        <v>1.57588392371526</v>
+        <v>1.6330165199336</v>
       </c>
       <c r="O29" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$24:K29)) * 20 + (SUM($M$3:$M$5) + SUM($M$24:M29)) * 1000) /(SUM($G$3:$G$5) + SUM($G$24:G29))</f>
-        <v>112.89459815735766</v>
+        <v>112.53202072250498</v>
       </c>
       <c r="P29" s="20">
         <f t="shared" si="52"/>
-        <v>56.669410734518557</v>
+        <v>57.772150607823107</v>
       </c>
       <c r="Q29" s="18">
         <f t="shared" si="50"/>
-        <v>62.637644097176327</v>
+        <v>61.148275293530645</v>
       </c>
       <c r="S29" t="s">
         <v>55</v>
@@ -3423,16 +3423,16 @@
         <v>14828.549459375599</v>
       </c>
       <c r="Z29">
-        <v>-236.73542760277701</v>
+        <v>-242.50151599851301</v>
       </c>
       <c r="AA29">
-        <v>-144532.24208097099</v>
+        <v>-147012.741783423</v>
       </c>
       <c r="AB29">
-        <v>34.789645891475402</v>
+        <v>35.483222543958902</v>
       </c>
       <c r="AC29">
-        <v>112.894598157357</v>
+        <v>112.532020722505</v>
       </c>
       <c r="AD29">
         <v>1.86707612500538</v>
@@ -3441,13 +3441,13 @@
         <v>1.4335380625026899</v>
       </c>
       <c r="AF29">
-        <v>1.33813230135688</v>
+        <v>1.37276991040251</v>
       </c>
       <c r="AG29">
-        <v>1.38406480690433</v>
+        <v>1.4177589226188301</v>
       </c>
       <c r="AH29">
-        <v>1.57588392371526</v>
+        <v>1.6330165199336</v>
       </c>
       <c r="AI29" t="s">
         <v>63</v>
@@ -3473,23 +3473,23 @@
       <c r="Q30" s="14"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+      <c r="N31" s="24"/>
+      <c r="O31" s="24"/>
       <c r="P31" s="20"/>
       <c r="Q31" s="18"/>
     </row>
@@ -3497,11 +3497,11 @@
       <c r="A32" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="27" t="str">
+      <c r="B32" s="22" t="str">
         <f>T32</f>
         <v>[80,85)</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="23">
         <f>V32/1000</f>
         <v>1508.4970000000001</v>
       </c>
@@ -3527,39 +3527,39 @@
       </c>
       <c r="I32" s="17">
         <f t="shared" ref="I32:I37" si="57">-Z32</f>
-        <v>14745.176590473</v>
+        <v>14993.793511620101</v>
       </c>
       <c r="J32" s="19">
         <f t="shared" ref="J32:J37" si="58">AF32</f>
-        <v>1.2318096288212299</v>
+        <v>1.2432372723713501</v>
       </c>
       <c r="K32" s="17">
         <f t="shared" ref="K32:K37" si="59">AB32</f>
-        <v>1483.6802485298799</v>
+        <v>1498.5521129625399</v>
       </c>
       <c r="L32" s="19">
         <f t="shared" ref="L32:L37" si="60">AG32</f>
-        <v>1.2315426429835099</v>
+        <v>1.2403764649723701</v>
       </c>
       <c r="M32" s="20">
         <f t="shared" ref="M32:M37" si="61">-AA32/1000000</f>
-        <v>4.3993137026748199</v>
+        <v>4.4373989306821198</v>
       </c>
       <c r="N32" s="19">
         <f t="shared" ref="N32:N37" si="62">AH32</f>
-        <v>1.32223614796613</v>
+        <v>1.3373412209539499</v>
       </c>
       <c r="O32" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K32)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M32)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G32))</f>
-        <v>100.94094864528336</v>
+        <v>98.854630261095551</v>
       </c>
       <c r="P32" s="20">
         <f>(K32 * 20 + M32 * 1000) /G32</f>
-        <v>66.357702849512393</v>
+        <v>67.011139782032714</v>
       </c>
       <c r="Q32" s="18">
         <f t="shared" ref="Q32:Q37" si="63">E32/I32*1000</f>
-        <v>17.411573463000167</v>
+        <v>17.122866553481717</v>
       </c>
       <c r="S32" t="s">
         <v>51</v>
@@ -3583,16 +3583,16 @@
         <v>513473.45085986197</v>
       </c>
       <c r="Z32">
-        <v>-14745.176590473</v>
+        <v>-14993.793511620101</v>
       </c>
       <c r="AA32">
-        <v>-4399313.7026748201</v>
+        <v>-4437398.9306821199</v>
       </c>
       <c r="AB32">
-        <v>1483.6802485298799</v>
+        <v>1498.5521129625399</v>
       </c>
       <c r="AC32">
-        <v>100.940948645283</v>
+        <v>98.854630261095593</v>
       </c>
       <c r="AD32">
         <v>1.4178160833803599</v>
@@ -3601,13 +3601,13 @@
         <v>1.4178160833803599</v>
       </c>
       <c r="AF32">
-        <v>1.2318096288212299</v>
+        <v>1.2432372723713501</v>
       </c>
       <c r="AG32">
-        <v>1.2315426429835099</v>
+        <v>1.2403764649723701</v>
       </c>
       <c r="AH32">
-        <v>1.32223614796613</v>
+        <v>1.3373412209539499</v>
       </c>
       <c r="AI32" t="s">
         <v>64</v>
@@ -3617,8 +3617,8 @@
       <c r="A33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="17">
         <f t="shared" ref="D33:D37" si="64">W33/1000</f>
         <v>432.33263577457899</v>
@@ -3641,39 +3641,39 @@
       </c>
       <c r="I33" s="17">
         <f t="shared" si="57"/>
-        <v>4622.8660166333002</v>
+        <v>4579.8958977517204</v>
       </c>
       <c r="J33" s="19">
         <f t="shared" si="58"/>
-        <v>1.3044859273267599</v>
+        <v>1.3175347732039699</v>
       </c>
       <c r="K33" s="17">
         <f t="shared" si="59"/>
-        <v>605.76204268788001</v>
+        <v>599.73654430174201</v>
       </c>
       <c r="L33" s="19">
         <f t="shared" si="60"/>
-        <v>1.32607766461099</v>
+        <v>1.3365776909337499</v>
       </c>
       <c r="M33" s="20">
         <f t="shared" si="61"/>
-        <v>1.81561196155161</v>
+        <v>1.7897514454472101</v>
       </c>
       <c r="N33" s="19">
         <f t="shared" si="62"/>
-        <v>1.4552241193253701</v>
+        <v>1.4734022213829701</v>
       </c>
       <c r="O33" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K33)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M33)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G33))</f>
-        <v>100.12857540168434</v>
+        <v>98.133723673196229</v>
       </c>
       <c r="P33" s="20">
         <f t="shared" ref="P33:P37" si="65">(K33 * 20 + M33 * 1000) /G33</f>
-        <v>90.893055498752744</v>
+        <v>89.938048602458409</v>
       </c>
       <c r="Q33" s="18">
         <f t="shared" si="63"/>
-        <v>16.57699087594705</v>
+        <v>16.732521762356058</v>
       </c>
       <c r="S33" t="s">
         <v>52</v>
@@ -3697,16 +3697,16 @@
         <v>153266.415556911</v>
       </c>
       <c r="Z33">
-        <v>-4622.8660166333002</v>
+        <v>-4579.8958977517204</v>
       </c>
       <c r="AA33">
-        <v>-1815611.9615516099</v>
+        <v>-1789751.44544721</v>
       </c>
       <c r="AB33">
-        <v>605.76204268788001</v>
+        <v>599.73654430174201</v>
       </c>
       <c r="AC33">
-        <v>100.128575401684</v>
+        <v>98.133723673196201</v>
       </c>
       <c r="AD33">
         <v>1.54252978251027</v>
@@ -3715,13 +3715,13 @@
         <v>1.54252978251027</v>
       </c>
       <c r="AF33">
-        <v>1.3044859273267599</v>
+        <v>1.3175347732039699</v>
       </c>
       <c r="AG33">
-        <v>1.32607766461099</v>
+        <v>1.3365776909337499</v>
       </c>
       <c r="AH33">
-        <v>1.4552241193253701</v>
+        <v>1.4734022213829701</v>
       </c>
       <c r="AI33" t="s">
         <v>64</v>
@@ -3731,11 +3731,11 @@
       <c r="A34" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="27" t="str">
+      <c r="B34" s="22" t="str">
         <f>T34</f>
         <v>[85,90)</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="23">
         <f>V34/1000</f>
         <v>940.56899999999996</v>
       </c>
@@ -3761,39 +3761,39 @@
       </c>
       <c r="I34" s="17">
         <f t="shared" si="57"/>
-        <v>2418.0540310684501</v>
+        <v>2446.1601279562801</v>
       </c>
       <c r="J34" s="19">
         <f t="shared" si="58"/>
-        <v>1.3425002707951099</v>
+        <v>1.3572176804580001</v>
       </c>
       <c r="K34" s="17">
         <f t="shared" si="59"/>
-        <v>208.27752535254399</v>
+        <v>210.052717532841</v>
       </c>
       <c r="L34" s="19">
         <f t="shared" si="60"/>
-        <v>1.3585813855050199</v>
+        <v>1.3702713671573701</v>
       </c>
       <c r="M34" s="20">
         <f t="shared" si="61"/>
-        <v>0.72091459386456902</v>
+        <v>0.72697001475812495</v>
       </c>
       <c r="N34" s="19">
         <f t="shared" si="62"/>
-        <v>1.5080288878505701</v>
+        <v>1.52866814545388</v>
       </c>
       <c r="O34" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K34)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M34)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G34))</f>
-        <v>97.864988233756407</v>
+        <v>95.985057498780066</v>
       </c>
       <c r="P34" s="20">
         <f t="shared" si="65"/>
-        <v>52.107114041916844</v>
+        <v>52.550283754592733</v>
       </c>
       <c r="Q34" s="18">
         <f t="shared" si="63"/>
-        <v>19.391070461363224</v>
+        <v>19.168269305005097</v>
       </c>
       <c r="S34" t="s">
         <v>53</v>
@@ -3817,16 +3817,16 @@
         <v>93777.312191663499</v>
       </c>
       <c r="Z34">
-        <v>-2418.0540310684501</v>
+        <v>-2446.1601279562801</v>
       </c>
       <c r="AA34">
-        <v>-720914.59386456897</v>
+        <v>-726970.01475812495</v>
       </c>
       <c r="AB34">
-        <v>208.27752535254399</v>
+        <v>210.052717532841</v>
       </c>
       <c r="AC34">
-        <v>97.864988233756307</v>
+        <v>95.985057498779994</v>
       </c>
       <c r="AD34">
         <v>1.6188368812010501</v>
@@ -3835,13 +3835,13 @@
         <v>1.6188368812010501</v>
       </c>
       <c r="AF34">
-        <v>1.3425002707951099</v>
+        <v>1.3572176804580001</v>
       </c>
       <c r="AG34">
-        <v>1.3585813855050199</v>
+        <v>1.3702713671573701</v>
       </c>
       <c r="AH34">
-        <v>1.5080288878505701</v>
+        <v>1.52866814545388</v>
       </c>
       <c r="AI34" t="s">
         <v>64</v>
@@ -3851,8 +3851,8 @@
       <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="28"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="17">
         <f t="shared" si="64"/>
         <v>595.70287520163299</v>
@@ -3875,39 +3875,39 @@
       </c>
       <c r="I35" s="17">
         <f t="shared" si="57"/>
-        <v>3441.1441042000301</v>
+        <v>3421.9017297001901</v>
       </c>
       <c r="J35" s="19">
         <f t="shared" si="58"/>
-        <v>1.39659866240273</v>
+        <v>1.41272958559462</v>
       </c>
       <c r="K35" s="17">
         <f t="shared" si="59"/>
-        <v>492.49389436391402</v>
+        <v>489.89476123665298</v>
       </c>
       <c r="L35" s="19">
         <f t="shared" si="60"/>
-        <v>1.435439817817</v>
+        <v>1.44885333297353</v>
       </c>
       <c r="M35" s="20">
         <f t="shared" si="61"/>
-        <v>1.7376057270065899</v>
+        <v>1.71789924427458</v>
       </c>
       <c r="N35" s="19">
         <f t="shared" si="62"/>
-        <v>1.63530314333593</v>
+        <v>1.65926677712804</v>
       </c>
       <c r="O35" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K35)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M35)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G35))</f>
-        <v>95.88248507092699</v>
+        <v>94.110775783860802</v>
       </c>
       <c r="P35" s="20">
         <f t="shared" si="65"/>
-        <v>71.533947681146856</v>
+        <v>71.091383295446619</v>
       </c>
       <c r="Q35" s="18">
         <f t="shared" si="63"/>
-        <v>23.536619407027647</v>
+        <v>23.668972841131058</v>
       </c>
       <c r="S35" t="s">
         <v>54</v>
@@ -3931,16 +3931,16 @@
         <v>161985.79821058601</v>
       </c>
       <c r="Z35">
-        <v>-3441.1441042000301</v>
+        <v>-3421.9017297001901</v>
       </c>
       <c r="AA35">
-        <v>-1737605.72700659</v>
+        <v>-1717899.2442745799</v>
       </c>
       <c r="AB35">
-        <v>492.49389436391402</v>
+        <v>489.89476123665298</v>
       </c>
       <c r="AC35">
-        <v>95.882485070926904</v>
+        <v>94.110775783860703</v>
       </c>
       <c r="AD35">
         <v>1.7506455884638199</v>
@@ -3949,13 +3949,13 @@
         <v>1.7506455884638199</v>
       </c>
       <c r="AF35">
-        <v>1.39659866240273</v>
+        <v>1.41272958559462</v>
       </c>
       <c r="AG35">
-        <v>1.435439817817</v>
+        <v>1.44885333297353</v>
       </c>
       <c r="AH35">
-        <v>1.63530314333593</v>
+        <v>1.65926677712804</v>
       </c>
       <c r="AI35" t="s">
         <v>64</v>
@@ -3995,39 +3995,39 @@
       </c>
       <c r="I36" s="17">
         <f t="shared" si="57"/>
-        <v>1689.26682976081</v>
+        <v>1687.40184965618</v>
       </c>
       <c r="J36" s="19">
         <f t="shared" si="58"/>
-        <v>1.4231557073037699</v>
+        <v>1.4401035135459801</v>
       </c>
       <c r="K36" s="17">
         <f t="shared" si="59"/>
-        <v>254.78764804356101</v>
+        <v>254.776716327858</v>
       </c>
       <c r="L36" s="19">
         <f t="shared" si="60"/>
-        <v>1.4752018928907999</v>
+        <v>1.48972099843435</v>
       </c>
       <c r="M36" s="20">
         <f t="shared" si="61"/>
-        <v>1.0054838530916901</v>
+        <v>1.0028080909625301</v>
       </c>
       <c r="N36" s="19">
         <f t="shared" si="62"/>
-        <v>1.70895173162947</v>
+        <v>1.7355025429612001</v>
       </c>
       <c r="O36" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K36)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M36)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G36))</f>
-        <v>93.774341360512011</v>
+        <v>92.090084943841546</v>
       </c>
       <c r="P36" s="20">
         <f t="shared" si="65"/>
-        <v>53.788679611625348</v>
+        <v>53.763162529154933</v>
       </c>
       <c r="Q36" s="18">
         <f t="shared" si="63"/>
-        <v>33.573664677645795</v>
+        <v>33.610771556885069</v>
       </c>
       <c r="S36" t="s">
         <v>54</v>
@@ -4051,16 +4051,16 @@
         <v>113429.75618691801</v>
       </c>
       <c r="Z36">
-        <v>-1689.26682976081</v>
+        <v>-1687.40184965618</v>
       </c>
       <c r="AA36">
-        <v>-1005483.85309169</v>
+        <v>-1002808.09096253</v>
       </c>
       <c r="AB36">
-        <v>254.78764804356101</v>
+        <v>254.776716327858</v>
       </c>
       <c r="AC36">
-        <v>93.774341360511897</v>
+        <v>92.090084943841504</v>
       </c>
       <c r="AD36">
         <v>1.8429439855658301</v>
@@ -4069,13 +4069,13 @@
         <v>1.8429439855658301</v>
       </c>
       <c r="AF36">
-        <v>1.4231557073037699</v>
+        <v>1.4401035135459801</v>
       </c>
       <c r="AG36">
-        <v>1.4752018928907999</v>
+        <v>1.48972099843435</v>
       </c>
       <c r="AH36">
-        <v>1.70895173162947</v>
+        <v>1.7355025429612001</v>
       </c>
       <c r="AI36" t="s">
         <v>64</v>
@@ -4115,39 +4115,39 @@
       </c>
       <c r="I37" s="17">
         <f t="shared" si="57"/>
-        <v>275.50396614288502</v>
+        <v>277.23480019250798</v>
       </c>
       <c r="J37" s="19">
         <f t="shared" si="58"/>
-        <v>1.42748691837733</v>
+        <v>1.4446009635444099</v>
       </c>
       <c r="K37" s="17">
         <f t="shared" si="59"/>
-        <v>40.389101170818698</v>
+        <v>40.5672077956918</v>
       </c>
       <c r="L37" s="19">
         <f t="shared" si="60"/>
-        <v>1.4815050025009</v>
+        <v>1.4962282142457899</v>
       </c>
       <c r="M37" s="20">
         <f t="shared" si="61"/>
-        <v>0.167633713289075</v>
+        <v>0.16826237552079701</v>
       </c>
       <c r="N37" s="19">
         <f t="shared" si="62"/>
-        <v>1.7212303836398199</v>
+        <v>1.7482942337885301</v>
       </c>
       <c r="O37" s="20">
         <f>((SUM($K$3:$K$5)+ SUM($K$32:K37)) * 20 + (SUM($M$3:$M$5) + SUM($M$32:M37)) * 1000) /(SUM($G$3:$G$5) + SUM($G$32:G37))</f>
-        <v>92.987402639204063</v>
+        <v>91.326741823223799</v>
       </c>
       <c r="P37" s="20">
         <f t="shared" si="65"/>
-        <v>32.889789368059951</v>
+        <v>33.03109768485335</v>
       </c>
       <c r="Q37" s="18">
         <f t="shared" si="63"/>
-        <v>53.823361118819783</v>
+        <v>53.487330771890328</v>
       </c>
       <c r="S37" t="s">
         <v>55</v>
@@ -4171,16 +4171,16 @@
         <v>29657.098918751301</v>
       </c>
       <c r="Z37">
-        <v>-275.50396614288502</v>
+        <v>-277.23480019250798</v>
       </c>
       <c r="AA37">
-        <v>-167633.71328907501</v>
+        <v>-168262.37552079701</v>
       </c>
       <c r="AB37">
-        <v>40.389101170818698</v>
+        <v>40.5672077956918</v>
       </c>
       <c r="AC37">
-        <v>92.987402639204007</v>
+        <v>91.326741823223699</v>
       </c>
       <c r="AD37">
         <v>1.86707612500538</v>
@@ -4189,13 +4189,13 @@
         <v>1.86707612500538</v>
       </c>
       <c r="AF37">
-        <v>1.42748691837733</v>
+        <v>1.4446009635444099</v>
       </c>
       <c r="AG37">
-        <v>1.4815050025009</v>
+        <v>1.4962282142457899</v>
       </c>
       <c r="AH37">
-        <v>1.7212303836398199</v>
+        <v>1.7482942337885301</v>
       </c>
       <c r="AI37" t="s">
         <v>64</v>
@@ -4203,6 +4203,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A15:O15"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:O7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="B16:B17"/>
@@ -4217,18 +4229,6 @@
     <mergeCell ref="A31:O31"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A15:O15"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:O7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>